<commit_message>
updating missing groups genotype
</commit_message>
<xml_diff>
--- a/data/raw/Cell_Counts/Dazl_100nMRA/241009_Dazl_100nMRA.xlsx
+++ b/data/raw/Cell_Counts/Dazl_100nMRA/241009_Dazl_100nMRA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umhealth-my.sharepoint.com/personal/kbonefas_med_umich_edu/Documents/Desktop/Cell_Counts/Dazl_100nMRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umhealth-my.sharepoint.com/personal/kbonefas_med_umich_edu/Documents/Documents/KDM5C_Germ_Mechanism/data/raw/Cell_Counts/Dazl_100nMRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="496" documentId="11_F25DC773A252ABDACC1048D6E9986E465BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5131920-9BC5-4936-9B2F-E589B32CCB75}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="11_F25DC773A252ABDACC1048D6E9986E465BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4DF3129-7585-4282-8E80-6483899DBAB4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="340" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="15">
   <si>
     <t>Image</t>
   </si>
@@ -128,10 +128,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2041,6 +2037,9 @@
       <c r="E82">
         <v>9</v>
       </c>
+      <c r="F82" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -2058,6 +2057,9 @@
       <c r="E83">
         <v>6</v>
       </c>
+      <c r="F83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -2075,6 +2077,9 @@
       <c r="E84">
         <v>2</v>
       </c>
+      <c r="F84" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
@@ -2092,6 +2097,9 @@
       <c r="E85">
         <v>10</v>
       </c>
+      <c r="F85" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -2109,6 +2117,9 @@
       <c r="E86">
         <v>11</v>
       </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -2126,6 +2137,9 @@
       <c r="E87">
         <v>6</v>
       </c>
+      <c r="F87" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -2143,6 +2157,9 @@
       <c r="E88">
         <v>5</v>
       </c>
+      <c r="F88" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
@@ -2160,6 +2177,9 @@
       <c r="E89">
         <v>17</v>
       </c>
+      <c r="F89" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -2177,6 +2197,9 @@
       <c r="E90">
         <v>3</v>
       </c>
+      <c r="F90" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
@@ -2193,6 +2216,9 @@
       </c>
       <c r="E91">
         <v>18</v>
+      </c>
+      <c r="F91" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>